<commit_message>
update portafolio de inversion
</commit_message>
<xml_diff>
--- a/Financial_proyect/Portafolio_Inversion.xlsx
+++ b/Financial_proyect/Portafolio_Inversion.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -82,13 +86,116 @@
   <si>
     <t>Var % Oro</t>
   </si>
+  <si>
+    <t>Indicadores</t>
+  </si>
+  <si>
+    <t>Rentabilidad Diaria</t>
+  </si>
+  <si>
+    <t>Rentabilidad Anual</t>
+  </si>
+  <si>
+    <t>Riesgo diario</t>
+  </si>
+  <si>
+    <t>Riesgo Anual</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Coeficiente de Correlación</t>
+  </si>
+  <si>
+    <t>Riesgo Sistemático</t>
+  </si>
+  <si>
+    <t>Riesgo No sistemático</t>
+  </si>
+  <si>
+    <t>Tasa Libre de Riesgo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Índice de Sharpe </t>
+  </si>
+  <si>
+    <t>Índice de Treynor</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Var % Cisco</t>
+  </si>
+  <si>
+    <t>Var % IBM</t>
+  </si>
+  <si>
+    <t>Var % Tesla</t>
+  </si>
+  <si>
+    <t>Var % Microsoft</t>
+  </si>
+  <si>
+    <t>Rentabilidad</t>
+  </si>
+  <si>
+    <t>Riesgo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riesgo </t>
+  </si>
+  <si>
+    <t>Índice de Sharpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beta </t>
+  </si>
+  <si>
+    <t>Acción</t>
+  </si>
+  <si>
+    <t>Máx Rentabilidad</t>
+  </si>
+  <si>
+    <t>Min Riesgo</t>
+  </si>
+  <si>
+    <t>RENT 17,82%</t>
+  </si>
+  <si>
+    <t>RENT 29,89%</t>
+  </si>
+  <si>
+    <t>RENT 41,96%</t>
+  </si>
+  <si>
+    <t>RENT 54,02%</t>
+  </si>
+  <si>
+    <t>RENT 66,09%</t>
+  </si>
+  <si>
+    <t>RENT 78,16%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="8">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.0000000%"/>
+    <numFmt numFmtId="170" formatCode="0.00000%"/>
+    <numFmt numFmtId="171" formatCode="0.000000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -131,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -165,12 +272,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,8 +395,145 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -200,6 +548,103 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Portafolio"/>
+      <sheetName val="Microsoft"/>
+      <sheetName val="Tesla"/>
+      <sheetName val="Cisco"/>
+      <sheetName val="IBM"/>
+      <sheetName val="Google"/>
+      <sheetName val="VaR de Tesla"/>
+      <sheetName val="EWMA - Tesla"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="26">
+          <cell r="V26" t="str">
+            <v>Rentabilidad</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="U27">
+            <v>1.5778894278876021E-2</v>
+          </cell>
+          <cell r="V27">
+            <v>5.759800833148887E-2</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="U28">
+            <v>1.73466433670455E-2</v>
+          </cell>
+          <cell r="V28">
+            <v>0.1782677108747473</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="U29">
+            <v>2.0503972955245999E-2</v>
+          </cell>
+          <cell r="V29">
+            <v>0.29893741341800573</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="U30">
+            <v>2.4452630439297147E-2</v>
+          </cell>
+          <cell r="V30">
+            <v>0.41960711596126415</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="U31">
+            <v>2.9066290699926788E-2</v>
+          </cell>
+          <cell r="V31">
+            <v>0.54027681850452258</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="U32">
+            <v>3.4016121309713987E-2</v>
+          </cell>
+          <cell r="V32">
+            <v>0.66094652104778107</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="U33">
+            <v>3.9171752607492311E-2</v>
+          </cell>
+          <cell r="V33">
+            <v>0.78161622359103955</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="U34">
+            <v>4.4586756208208136E-2</v>
+          </cell>
+          <cell r="V34">
+            <v>0.90228592613429803</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,6 +1021,7 @@
       <c r="J2" s="3">
         <v>1710.85</v>
       </c>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -17580,4 +18026,2195 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="10" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E3" s="10" t="e">
+        <f t="shared" ref="E3:I3" si="0">AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F3" s="10" t="e">
+        <f t="shared" ref="F3:J3" si="1">AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G3" s="10" t="e">
+        <f t="shared" ref="G3:K3" si="2">AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H3" s="10" t="e">
+        <f t="shared" ref="H3:K3" si="3">AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I3" s="10" t="e">
+        <f t="shared" ref="I3:L3" si="4">AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J3" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K3" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L3" s="10" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="12" t="e">
+        <f>(1+D3)^270-1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E4" s="12" t="e">
+        <f t="shared" ref="E4:I4" si="5">(1+E3)^270-1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F4" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G4" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H4" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="I4" s="12" t="e">
+        <f t="shared" si="5"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J4" s="12" t="e">
+        <f t="shared" ref="J4:L4" si="6">(1+J3)^270-1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K4" s="12" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L4" s="12" t="e">
+        <f t="shared" si="6"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="12" t="e">
+        <f>_xlfn.STDEV.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E5" s="12" t="e">
+        <f t="shared" ref="E5:I5" si="7">_xlfn.STDEV.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F5" s="12" t="e">
+        <f t="shared" ref="F5:J5" si="8">_xlfn.STDEV.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G5" s="12" t="e">
+        <f t="shared" ref="G5:K5" si="9">_xlfn.STDEV.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H5" s="12" t="e">
+        <f t="shared" ref="H5:K5" si="10">_xlfn.STDEV.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I5" s="12" t="e">
+        <f t="shared" ref="I5:L5" si="11">_xlfn.STDEV.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J5" s="12" t="e">
+        <f t="shared" si="11"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K5" s="12" t="e">
+        <f t="shared" si="11"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L5" s="12" t="e">
+        <f t="shared" si="11"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="12" t="e">
+        <f>D5*SQRT(270)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E6" s="12" t="e">
+        <f t="shared" ref="E6:I6" si="12">E5*SQRT(270)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F6" s="12" t="e">
+        <f t="shared" si="12"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G6" s="12" t="e">
+        <f t="shared" si="12"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H6" s="12" t="e">
+        <f t="shared" si="12"/>
+        <v>#REF!</v>
+      </c>
+      <c r="I6" s="12" t="e">
+        <f t="shared" si="12"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J6" s="12" t="e">
+        <f t="shared" ref="J6:L6" si="13">J5*SQRT(270)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K6" s="12" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L6" s="12" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="13" t="e">
+        <f>ABS(D6/D4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E7" s="13" t="e">
+        <f>ABS(E6/E4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F7" s="13" t="e">
+        <f t="shared" ref="F7:I7" si="14">ABS(F6/F4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G7" s="13" t="e">
+        <f t="shared" si="14"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H7" s="13" t="e">
+        <f t="shared" si="14"/>
+        <v>#REF!</v>
+      </c>
+      <c r="I7" s="13" t="e">
+        <f t="shared" si="14"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J7" s="13" t="e">
+        <f t="shared" ref="J7:L7" si="15">ABS(J6/J4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K7" s="13" t="e">
+        <f t="shared" si="15"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L7" s="13" t="e">
+        <f t="shared" si="15"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="14" t="e">
+        <f>_xlfn.COVARIANCE.P($I$4:$I$866,#REF!)/_xlfn.VAR.P($I$4:$I$866)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E8" s="14" t="e">
+        <f t="shared" ref="E8:I8" si="16">_xlfn.COVARIANCE.P($I$4:$I$866,#REF!)/_xlfn.VAR.P($I$4:$I$866)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F8" s="14" t="e">
+        <f t="shared" ref="F8:J8" si="17">_xlfn.COVARIANCE.P($I$4:$I$866,#REF!)/_xlfn.VAR.P($I$4:$I$866)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G8" s="14" t="e">
+        <f t="shared" ref="G8:K8" si="18">_xlfn.COVARIANCE.P($I$4:$I$866,#REF!)/_xlfn.VAR.P($I$4:$I$866)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H8" s="14" t="e">
+        <f t="shared" ref="H8:K8" si="19">_xlfn.COVARIANCE.P($I$4:$I$866,#REF!)/_xlfn.VAR.P($I$4:$I$866)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I8" s="14" t="e">
+        <f t="shared" ref="I8:L8" si="20">_xlfn.COVARIANCE.P($I$4:$I$866,#REF!)/_xlfn.VAR.P($I$4:$I$866)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J8" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K8" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L8" s="14" t="e">
+        <f t="shared" si="20"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="15" t="e">
+        <f>CORREL($I$4:$I$866,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E9" s="15" t="e">
+        <f>CORREL($I$4:$I$866,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F9" s="15" t="e">
+        <f>CORREL($I$4:$I$866,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G9" s="15" t="e">
+        <f>CORREL($I$4:$I$866,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H9" s="15" t="e">
+        <f t="shared" ref="H9:I9" si="21">CORREL($I$4:$I$866,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I9" s="15" t="e">
+        <f t="shared" ref="I9:L9" si="22">CORREL($I$4:$I$866,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J9" s="15" t="e">
+        <f t="shared" si="22"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K9" s="15" t="e">
+        <f t="shared" si="22"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L9" s="15" t="e">
+        <f t="shared" si="22"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="13" t="e">
+        <f>D8^2*_xlfn.VAR.P($I$4:$I$866)/_xlfn.VAR.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E10" s="13" t="e">
+        <f>E8^2*_xlfn.VAR.P($I$4:$I$866)/_xlfn.VAR.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F10" s="13" t="e">
+        <f t="shared" ref="F10:I10" si="23">F8^2*_xlfn.VAR.P($I$4:$I$866)/_xlfn.VAR.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G10" s="13" t="e">
+        <f t="shared" ref="G10:J10" si="24">G8^2*_xlfn.VAR.P($I$4:$I$866)/_xlfn.VAR.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H10" s="13" t="e">
+        <f t="shared" ref="H10:K10" si="25">H8^2*_xlfn.VAR.P($I$4:$I$866)/_xlfn.VAR.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I10" s="13" t="e">
+        <f t="shared" ref="I10:L10" si="26">I8^2*_xlfn.VAR.P($I$4:$I$866)/_xlfn.VAR.P(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J10" s="13" t="e">
+        <f t="shared" si="26"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K10" s="13" t="e">
+        <f t="shared" si="26"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L10" s="13" t="e">
+        <f t="shared" si="26"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="16" t="e">
+        <f>1-D10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E11" s="16" t="e">
+        <f>1-E10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F11" s="16" t="e">
+        <f>1-F10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G11" s="16" t="e">
+        <f t="shared" ref="G11:I11" si="27">1-G10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H11" s="16" t="e">
+        <f t="shared" si="27"/>
+        <v>#REF!</v>
+      </c>
+      <c r="I11" s="16" t="e">
+        <f t="shared" si="27"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J11" s="16" t="e">
+        <f t="shared" ref="J11:L11" si="28">1-J10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K11" s="16" t="e">
+        <f t="shared" si="28"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L11" s="16" t="e">
+        <f t="shared" si="28"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="17">
+        <v>3.8989999999999997E-2</v>
+      </c>
+      <c r="E12" s="17">
+        <v>3.8989999999999997E-2</v>
+      </c>
+      <c r="F12" s="17">
+        <v>3.8989999999999997E-2</v>
+      </c>
+      <c r="G12" s="17">
+        <v>3.8989999999999997E-2</v>
+      </c>
+      <c r="H12" s="17">
+        <v>3.8989999999999997E-2</v>
+      </c>
+      <c r="I12" s="17">
+        <v>3.8989999999999997E-2</v>
+      </c>
+      <c r="J12" s="17">
+        <v>1.0389900000000001</v>
+      </c>
+      <c r="K12" s="17">
+        <v>2.0389900000000001</v>
+      </c>
+      <c r="L12" s="17">
+        <v>3.0389900000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="17" t="e">
+        <f>(D4-D12)/D6</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E13" s="17" t="e">
+        <f>(E4-E12)/E6</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F13" s="17" t="e">
+        <f>(F4-F12)/F6</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G13" s="17" t="e">
+        <f t="shared" ref="G13:I13" si="29">(G4-G12)/G6</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H13" s="17" t="e">
+        <f t="shared" si="29"/>
+        <v>#REF!</v>
+      </c>
+      <c r="I13" s="17" t="e">
+        <f t="shared" si="29"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J13" s="17" t="e">
+        <f t="shared" ref="J13:L13" si="30">(J4-J12)/J6</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K13" s="17" t="e">
+        <f t="shared" si="30"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L13" s="17" t="e">
+        <f t="shared" si="30"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="19" t="e">
+        <f>(D4-D12)/D8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E14" s="19" t="e">
+        <f t="shared" ref="E14:I14" si="31">(E4-E12)/E8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F14" s="19" t="e">
+        <f t="shared" si="31"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G14" s="19" t="e">
+        <f t="shared" si="31"/>
+        <v>#REF!</v>
+      </c>
+      <c r="H14" s="19" t="e">
+        <f t="shared" si="31"/>
+        <v>#REF!</v>
+      </c>
+      <c r="I14" s="19" t="e">
+        <f t="shared" si="31"/>
+        <v>#REF!</v>
+      </c>
+      <c r="J14" s="19" t="e">
+        <f t="shared" ref="J14:L14" si="32">(J4-J12)/J8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K14" s="19" t="e">
+        <f t="shared" si="32"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L14" s="19" t="e">
+        <f t="shared" si="32"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="20">
+        <f>B19</f>
+        <v>4.2309967829213889E-2</v>
+      </c>
+      <c r="E16" s="20">
+        <f>B20</f>
+        <v>3.6602161261712639E-2</v>
+      </c>
+      <c r="F16" s="20">
+        <f>B21</f>
+        <v>3.6225611297570869E-2</v>
+      </c>
+      <c r="G16" s="20">
+        <f>B22</f>
+        <v>1.3392085615291665E-2</v>
+      </c>
+      <c r="H16" s="20">
+        <f>B23</f>
+        <v>0.85133436836981968</v>
+      </c>
+      <c r="I16" s="20">
+        <f>B24</f>
+        <v>2.0135801036845504E-2</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="21">
+        <f>SUM(B19:B24)</f>
+        <v>0.99999999541045426</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="11">
+        <v>3.2386102818871909E-4</v>
+      </c>
+      <c r="E18" s="11">
+        <v>2.3039325985357105E-4</v>
+      </c>
+      <c r="F18" s="11">
+        <v>1.7699553495874524E-4</v>
+      </c>
+      <c r="G18" s="22">
+        <v>3.2828247275174807E-4</v>
+      </c>
+      <c r="H18" s="11">
+        <v>5.0359077952696093E-4</v>
+      </c>
+      <c r="I18" s="6">
+        <v>3.4454689956896298E-4</v>
+      </c>
+      <c r="J18" s="23" t="e">
+        <f>D4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K18" s="24" t="e">
+        <f>D8</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="25">
+        <v>4.2309967829213889E-2</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2.3039325985357105E-4</v>
+      </c>
+      <c r="E19" s="11">
+        <v>3.6939866058534663E-4</v>
+      </c>
+      <c r="F19" s="11">
+        <v>2.1424890987187991E-4</v>
+      </c>
+      <c r="G19" s="26">
+        <v>2.319242335731307E-4</v>
+      </c>
+      <c r="H19" s="11">
+        <v>2.3960956466516253E-4</v>
+      </c>
+      <c r="I19" s="6">
+        <v>2.534710055511346E-4</v>
+      </c>
+      <c r="J19" s="23" t="e">
+        <f>E4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K19" s="24" t="e">
+        <f>E8</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="25">
+        <v>3.6602161261712639E-2</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="11">
+        <v>1.7699553495874524E-4</v>
+      </c>
+      <c r="E20" s="11">
+        <v>2.1424890987187991E-4</v>
+      </c>
+      <c r="F20" s="11">
+        <v>3.4202845978806957E-4</v>
+      </c>
+      <c r="G20" s="26">
+        <v>1.7158508959452546E-4</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1.7398076653148335E-4</v>
+      </c>
+      <c r="I20" s="6">
+        <v>1.8127983112415619E-4</v>
+      </c>
+      <c r="J20" s="23" t="e">
+        <f>F4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K20" s="27" t="e">
+        <f>F8</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="25">
+        <v>3.6225611297570869E-2</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="11">
+        <v>3.2828247275174807E-4</v>
+      </c>
+      <c r="E21" s="11">
+        <v>2.319242335731307E-4</v>
+      </c>
+      <c r="F21" s="11">
+        <v>1.7158508959452546E-4</v>
+      </c>
+      <c r="G21" s="26">
+        <v>4.7340096400834203E-4</v>
+      </c>
+      <c r="H21" s="11">
+        <v>4.2787215289800848E-4</v>
+      </c>
+      <c r="I21" s="6">
+        <v>3.7817165286242244E-4</v>
+      </c>
+      <c r="J21" s="23" t="e">
+        <f>G4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K21" s="27" t="e">
+        <f>G8</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="25">
+        <v>1.3392085615291665E-2</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="11">
+        <v>5.0359077952696093E-4</v>
+      </c>
+      <c r="E22" s="11">
+        <v>2.3960956466516253E-4</v>
+      </c>
+      <c r="F22" s="11">
+        <v>1.7398076653148335E-4</v>
+      </c>
+      <c r="G22" s="26">
+        <v>4.2787215289800848E-4</v>
+      </c>
+      <c r="H22" s="11">
+        <v>1.9879788291701848E-3</v>
+      </c>
+      <c r="I22" s="6">
+        <v>4.691410725479059E-4</v>
+      </c>
+      <c r="J22" s="23" t="e">
+        <f>H4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K22" s="24" t="e">
+        <f>H8</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="25">
+        <v>0.85133436836981968</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="18">
+        <v>3.4454689956896293E-4</v>
+      </c>
+      <c r="E23" s="18">
+        <v>2.534710055511346E-4</v>
+      </c>
+      <c r="F23" s="18">
+        <v>1.8127983112415619E-4</v>
+      </c>
+      <c r="G23" s="28">
+        <v>3.7817165286242244E-4</v>
+      </c>
+      <c r="H23" s="18">
+        <v>4.691410725479059E-4</v>
+      </c>
+      <c r="I23" s="29">
+        <v>4.6203795124722167E-4</v>
+      </c>
+      <c r="J23" s="30" t="e">
+        <f>I4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K23" s="31" t="e">
+        <f>I8</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="25">
+        <v>2.0135801036845504E-2</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6">
+        <f>SUMPRODUCT(D18:D23,$P$19:$P$24)*D16</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" ref="E24:I24" si="33">SUMPRODUCT(E18:E23,$P$19:$P$24)*E16</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="6">
+        <f>SUMPRODUCT(F18:F23,$P$19:$P$24)*F16</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="6">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="33" t="e">
+        <f>SUMPRODUCT(B19:B24,J18:J23)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="38">
+        <f>SQRT(SUM(D24:I24))</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="22">
+        <v>1</v>
+      </c>
+      <c r="G27" s="39">
+        <f>E44</f>
+        <v>1.5778894278876021E-2</v>
+      </c>
+      <c r="H27" s="40">
+        <f>+E43</f>
+        <v>5.759800833148887E-2</v>
+      </c>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="4" t="e">
+        <f>(D26-D12)/D27</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="26">
+        <v>2</v>
+      </c>
+      <c r="G28" s="41">
+        <v>1.73466433670455E-2</v>
+      </c>
+      <c r="H28" s="42">
+        <f t="shared" ref="H28:H34" si="34">H27+($R$43-$S$43)/7</f>
+        <v>5.759800833148887E-2</v>
+      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="11" t="e">
+        <f>SUMPRODUCT(B19:B24,K18:K23)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="26">
+        <v>3</v>
+      </c>
+      <c r="G29" s="41">
+        <v>2.0503972955245999E-2</v>
+      </c>
+      <c r="H29" s="42">
+        <f t="shared" si="34"/>
+        <v>5.759800833148887E-2</v>
+      </c>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="18" t="e">
+        <f>(D26-D12)/D29</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="26">
+        <v>4</v>
+      </c>
+      <c r="G30" s="41">
+        <v>2.4452630439297147E-2</v>
+      </c>
+      <c r="H30" s="42">
+        <f t="shared" si="34"/>
+        <v>5.759800833148887E-2</v>
+      </c>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="26">
+        <v>5</v>
+      </c>
+      <c r="G31" s="41">
+        <v>2.9066290699926788E-2</v>
+      </c>
+      <c r="H31" s="42">
+        <f t="shared" si="34"/>
+        <v>5.759800833148887E-2</v>
+      </c>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="26">
+        <v>6</v>
+      </c>
+      <c r="G32" s="41">
+        <v>3.4016121309713987E-2</v>
+      </c>
+      <c r="H32" s="42">
+        <f t="shared" si="34"/>
+        <v>5.759800833148887E-2</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="26">
+        <v>7</v>
+      </c>
+      <c r="G33" s="41">
+        <v>3.9171752607492311E-2</v>
+      </c>
+      <c r="H33" s="42">
+        <f t="shared" si="34"/>
+        <v>5.759800833148887E-2</v>
+      </c>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+    </row>
+    <row r="34" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="28">
+        <v>8</v>
+      </c>
+      <c r="G34" s="46">
+        <f>+D44</f>
+        <v>4.4586756208208136E-2</v>
+      </c>
+      <c r="H34" s="47">
+        <f t="shared" si="34"/>
+        <v>5.759800833148887E-2</v>
+      </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+    </row>
+    <row r="35" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+    </row>
+    <row r="36" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="H36" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="I36" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="J36" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="K36" s="48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="37" t="str">
+        <f t="shared" ref="C37:C42" si="35">MID(C18,6,20)</f>
+        <v xml:space="preserve"> Nasdaq</v>
+      </c>
+      <c r="D37" s="49">
+        <v>0</v>
+      </c>
+      <c r="E37" s="49">
+        <v>0.42421261791303044</v>
+      </c>
+      <c r="F37" s="49">
+        <v>0.24099802933843645</v>
+      </c>
+      <c r="G37" s="49">
+        <v>0.28297080893440879</v>
+      </c>
+      <c r="H37" s="49">
+        <v>0.1535807291527424</v>
+      </c>
+      <c r="I37" s="49">
+        <v>0.12256443897012619</v>
+      </c>
+      <c r="J37" s="49">
+        <v>8.5716918357413213E-2</v>
+      </c>
+      <c r="K37" s="49">
+        <v>4.2309967829213889E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="37" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve"> Cisco</v>
+      </c>
+      <c r="D38" s="16">
+        <v>0</v>
+      </c>
+      <c r="E38" s="16">
+        <v>0.18011915998551412</v>
+      </c>
+      <c r="F38" s="16">
+        <v>0.17942474721933963</v>
+      </c>
+      <c r="G38" s="16">
+        <v>0.17878207246460881</v>
+      </c>
+      <c r="H38" s="16">
+        <v>0.16982342632460842</v>
+      </c>
+      <c r="I38" s="16">
+        <v>0.12644081916252153</v>
+      </c>
+      <c r="J38" s="16">
+        <v>8.1580955944500738E-2</v>
+      </c>
+      <c r="K38" s="16">
+        <v>3.6602161261712639E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="37" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve"> IBM</v>
+      </c>
+      <c r="D39" s="16">
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
+        <v>0.39566822210145547</v>
+      </c>
+      <c r="F39" s="16">
+        <v>0.39240740840725546</v>
+      </c>
+      <c r="G39" s="16">
+        <v>0.21989030715449021</v>
+      </c>
+      <c r="H39" s="16">
+        <v>0.20670250563712311</v>
+      </c>
+      <c r="I39" s="16">
+        <v>0.14264936228729111</v>
+      </c>
+      <c r="J39" s="16">
+        <v>8.5744217607902393E-2</v>
+      </c>
+      <c r="K39" s="16">
+        <v>3.6225611297570869E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="37" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve"> Google</v>
+      </c>
+      <c r="D40" s="16">
+        <v>0</v>
+      </c>
+      <c r="E40" s="16">
+        <v>0</v>
+      </c>
+      <c r="F40" s="16">
+        <v>1.4960661921451306E-2</v>
+      </c>
+      <c r="G40" s="16">
+        <v>1.5238590738042835E-2</v>
+      </c>
+      <c r="H40" s="16">
+        <v>1.5284082960186123E-2</v>
+      </c>
+      <c r="I40" s="16">
+        <v>1.5007806890385205E-2</v>
+      </c>
+      <c r="J40" s="16">
+        <v>1.4510915062719782E-2</v>
+      </c>
+      <c r="K40" s="16">
+        <v>1.3392085615291665E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="37" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve"> Tesla</v>
+      </c>
+      <c r="D41" s="16">
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="E41" s="16">
+        <v>0</v>
+      </c>
+      <c r="F41" s="16">
+        <v>0.14869968381484253</v>
+      </c>
+      <c r="G41" s="16">
+        <v>0.27875851398962775</v>
+      </c>
+      <c r="H41" s="16">
+        <v>0.43006686945295353</v>
+      </c>
+      <c r="I41" s="16">
+        <v>0.56946200102008704</v>
+      </c>
+      <c r="J41" s="16">
+        <v>0.70974861655770316</v>
+      </c>
+      <c r="K41" s="16">
+        <v>0.85133436836981968</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="37" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve"> Microsoft</v>
+      </c>
+      <c r="D42" s="16">
+        <v>0</v>
+      </c>
+      <c r="E42" s="16">
+        <v>0</v>
+      </c>
+      <c r="F42" s="16">
+        <v>2.3509469298677657E-2</v>
+      </c>
+      <c r="G42" s="16">
+        <v>2.4359708736133728E-2</v>
+      </c>
+      <c r="H42" s="16">
+        <v>2.4542385649284862E-2</v>
+      </c>
+      <c r="I42" s="16">
+        <v>2.387556306412443E-2</v>
+      </c>
+      <c r="J42" s="16">
+        <v>2.269837225941156E-2</v>
+      </c>
+      <c r="K42" s="16">
+        <v>2.0135801036845504E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="50">
+        <v>0.90228592613429792</v>
+      </c>
+      <c r="E43" s="50">
+        <v>5.759800833148887E-2</v>
+      </c>
+      <c r="F43" s="50">
+        <v>0.17826771087474658</v>
+      </c>
+      <c r="G43" s="50">
+        <v>0.29893759168571682</v>
+      </c>
+      <c r="H43" s="50">
+        <v>0.41960741489885567</v>
+      </c>
+      <c r="I43" s="50">
+        <v>0.54027723811193784</v>
+      </c>
+      <c r="J43" s="50">
+        <v>0.6609470613250189</v>
+      </c>
+      <c r="K43" s="50">
+        <v>0.7816168845381013</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="50">
+        <v>4.4586756208208136E-2</v>
+      </c>
+      <c r="E44" s="50">
+        <v>1.5778894278876021E-2</v>
+      </c>
+      <c r="F44" s="50">
+        <v>1.73466433670455E-2</v>
+      </c>
+      <c r="G44" s="50">
+        <v>2.0503972955245999E-2</v>
+      </c>
+      <c r="H44" s="50">
+        <v>2.4452630439297147E-2</v>
+      </c>
+      <c r="I44" s="50">
+        <v>2.9066290699926788E-2</v>
+      </c>
+      <c r="J44" s="50">
+        <v>3.4016121309713987E-2</v>
+      </c>
+      <c r="K44" s="50">
+        <v>3.9171752607492311E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="11">
+        <v>19.362160416042347</v>
+      </c>
+      <c r="E45" s="11">
+        <v>1.1792973577622816</v>
+      </c>
+      <c r="F45" s="11">
+        <v>8.0290871223732516</v>
+      </c>
+      <c r="G45" s="11">
+        <v>12.677913312366529</v>
+      </c>
+      <c r="H45" s="11">
+        <v>15.565499828074772</v>
+      </c>
+      <c r="I45" s="11">
+        <v>17.24634365241522</v>
+      </c>
+      <c r="J45" s="11">
+        <v>18.284185185669791</v>
+      </c>
+      <c r="K45" s="11">
+        <v>18.958224616073483</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="11">
+        <v>1.5549594909379174</v>
+      </c>
+      <c r="E46" s="11">
+        <v>0.76858794980131817</v>
+      </c>
+      <c r="F46" s="11">
+        <v>0.85449524519357234</v>
+      </c>
+      <c r="G46" s="11">
+        <v>1.0051497943517274</v>
+      </c>
+      <c r="H46" s="11">
+        <v>1.0976980393798448</v>
+      </c>
+      <c r="I46" s="11">
+        <v>1.2165777534679831</v>
+      </c>
+      <c r="J46" s="11">
+        <v>1.3331014531775369</v>
+      </c>
+      <c r="K46" s="11">
+        <v>1.446933791355884</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="18">
+        <v>0.55518869215916156</v>
+      </c>
+      <c r="E47" s="18">
+        <v>2.4210642824024353E-2</v>
+      </c>
+      <c r="F47" s="18">
+        <v>0.1629941321009872</v>
+      </c>
+      <c r="G47" s="18">
+        <v>0.25861577363538168</v>
+      </c>
+      <c r="H47" s="18">
+        <v>0.34674145461158812</v>
+      </c>
+      <c r="I47" s="18">
+        <v>0.41204702016206179</v>
+      </c>
+      <c r="J47" s="18">
+        <v>0.46654893357331695</v>
+      </c>
+      <c r="K47" s="18">
+        <v>0.51324178685619404</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+    </row>
+    <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+    </row>
+    <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+    </row>
+    <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+    </row>
+    <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+    </row>
+    <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+    </row>
+    <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+    </row>
+    <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+    </row>
+    <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+    </row>
+    <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+    </row>
+    <row r="58" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+    </row>
+    <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+    </row>
+    <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="6"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+    </row>
+    <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+    </row>
+    <row r="62" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+    </row>
+    <row r="63" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="6"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+    </row>
+    <row r="64" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="6"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+    </row>
+    <row r="65" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="6"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+    </row>
+    <row r="66" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+    </row>
+    <row r="67" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+    </row>
+    <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+    </row>
+    <row r="69" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+    </row>
+    <row r="70" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+    </row>
+    <row r="71" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="6"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+    </row>
+    <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+    </row>
+    <row r="73" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="6"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+    </row>
+    <row r="74" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+    </row>
+    <row r="75" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+    </row>
+    <row r="76" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+    </row>
+    <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+    </row>
+    <row r="78" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+    </row>
+    <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+    </row>
+    <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="6"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+    </row>
+    <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="6"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+    </row>
+    <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="6"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+    </row>
+    <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="6"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+    </row>
+    <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="6"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+    </row>
+    <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="6"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+    </row>
+    <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="6"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+    </row>
+    <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="6"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+    </row>
+    <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="6"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+    </row>
+    <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="6"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+    </row>
+    <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="6"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+    </row>
+    <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="6"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+    </row>
+    <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="6"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+    </row>
+    <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="6"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+    </row>
+    <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="6"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+    </row>
+    <row r="95" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="6"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+    </row>
+    <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="6"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+    </row>
+    <row r="97" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="6"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+    </row>
+    <row r="98" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="6"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+    </row>
+    <row r="99" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="6"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+    </row>
+    <row r="100" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="6"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F26:G26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>